<commit_message>
added ev sales share data from bistline paper.
</commit_message>
<xml_diff>
--- a/data-extra/VariableMapping.xlsx
+++ b/data-extra/VariableMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcole\Documents\LEEP\LEEP\data-extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31D65118-449C-4075-A147-D276EA53DF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EA0DA-A3CC-4F43-BBDE-37FDDCD6F3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="4065" windowWidth="19620" windowHeight="13725" xr2:uid="{DA92EE2D-36A0-48E9-BFBF-9573E46ECB63}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18900" windowHeight="11160" xr2:uid="{DA92EE2D-36A0-48E9-BFBF-9573E46ECB63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>Bistline Variable</t>
   </si>
@@ -246,6 +244,15 @@
   </si>
   <si>
     <t>Power SO2</t>
+  </si>
+  <si>
+    <t>EV Sales Share (%)</t>
+  </si>
+  <si>
+    <t>Energy Service|Transportation|Passenger|BEV|Sales Share</t>
+  </si>
+  <si>
+    <t>Do all the models regard EV sales share as full BEVs? Or are there PHEVs in the mix too? Just linking BEV variable for now.</t>
   </si>
 </sst>
 </file>
@@ -600,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA515E4B-9157-4310-B5F6-E3E96B70C107}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,6 +963,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -963,6 +981,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1383,21 +1406,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -1439,7 +1448,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303F5059-C929-45FC-82ED-C8A8B8964CF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1462,23 +1488,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{490D51B6-E972-495C-9AF2-62BB75061D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1497,4 +1507,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>